<commit_message>
Just to make sure all is up to date.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\razmo\PycharmProjects\Streamlit_project\streamlit_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0470F741-F049-42ED-8AA3-7AAB7287DD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C77A5F-48CD-4FA7-8D89-44F30FD5385C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +386,9 @@
       <c r="C2">
         <v>0.2</v>
       </c>
+      <c r="D2">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -397,6 +400,9 @@
       <c r="C3">
         <v>0.2</v>
       </c>
+      <c r="D3">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -408,6 +414,9 @@
       <c r="C4">
         <v>0.2</v>
       </c>
+      <c r="D4">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -419,6 +428,9 @@
       <c r="C5">
         <v>0.2</v>
       </c>
+      <c r="D5">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -429,6 +441,51 @@
       </c>
       <c r="C6">
         <v>0.2</v>
+      </c>
+      <c r="D6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5.2</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>6.4</v>
+      </c>
+      <c r="C8">
+        <v>0.2</v>
+      </c>
+      <c r="D8">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>6.9</v>
+      </c>
+      <c r="C9">
+        <v>0.2</v>
+      </c>
+      <c r="D9">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>